<commit_message>
can generate micronaut contoller sources in case get request paramater
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtResourceBundle.xlsx
+++ b/meta/program/BlancoRestGeneratorKtResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C49C10-9E63-EA48-8D3B-5438AAF8BB2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE956E-BB86-9A41-8D5D-47DB8BF49F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="3840" windowWidth="25520" windowHeight="12280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="3840" windowWidth="25520" windowHeight="12280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="169">
   <si>
     <t>リソースバンドル定義書</t>
   </si>
@@ -933,6 +933,14 @@
     <rPh sb="52" eb="54">
       <t xml:space="preserve">ゼンテイ </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>META2XML.PROCESS_GET_REQUEST_BIND</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blancotelegramprocess-get-request-bind</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1800,10 +1808,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2377,10 +2385,10 @@
         <v>26</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
@@ -2395,10 +2403,10 @@
         <v>27</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25"/>
@@ -2407,22 +2415,23 @@
       <c r="H41" s="26"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" s="36" customFormat="1">
+    <row r="42" spans="1:9">
       <c r="A42" s="22">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B42" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="B42" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
       <c r="H42" s="26"/>
+      <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" s="36" customFormat="1">
       <c r="A43" s="22">
@@ -2430,10 +2439,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D43" s="41"/>
       <c r="E43" s="41"/>
@@ -2447,10 +2456,10 @@
         <v>30</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D44" s="41"/>
       <c r="E44" s="41"/>
@@ -2464,10 +2473,10 @@
         <v>31</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D45" s="41"/>
       <c r="E45" s="41"/>
@@ -2481,10 +2490,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D46" s="41"/>
       <c r="E46" s="41"/>
@@ -2498,10 +2507,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D47" s="41"/>
       <c r="E47" s="41"/>
@@ -2515,10 +2524,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" s="41"/>
       <c r="E48" s="41"/>
@@ -2532,30 +2541,33 @@
         <v>35</v>
       </c>
       <c r="B49" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" s="36" customFormat="1">
+      <c r="A50" s="22">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B50" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C50" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="22">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
       <c r="H50" s="26"/>
-      <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="22">
@@ -2563,9 +2575,7 @@
         <v>37</v>
       </c>
       <c r="B51" s="23"/>
-      <c r="C51" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="C51" s="24"/>
       <c r="D51" s="25"/>
       <c r="E51" s="25"/>
       <c r="F51" s="25"/>
@@ -2578,11 +2588,9 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B52" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="B52" s="23"/>
       <c r="C52" s="24" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
@@ -2597,10 +2605,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
@@ -2615,10 +2623,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25"/>
@@ -2633,10 +2641,10 @@
         <v>41</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
@@ -2651,10 +2659,10 @@
         <v>42</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="25"/>
@@ -2669,10 +2677,10 @@
         <v>43</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
@@ -2687,10 +2695,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25"/>
@@ -2705,10 +2713,10 @@
         <v>45</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25"/>
@@ -2723,10 +2731,10 @@
         <v>46</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
@@ -2740,8 +2748,12 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="24"/>
+      <c r="B61" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>148</v>
+      </c>
       <c r="D61" s="25"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
@@ -2754,12 +2766,8 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B62" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>41</v>
-      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="25"/>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
@@ -2773,10 +2781,10 @@
         <v>49</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="25"/>
@@ -2791,10 +2799,10 @@
         <v>50</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
@@ -2808,8 +2816,12 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="24"/>
+      <c r="B65" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
@@ -2822,12 +2834,8 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B66" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>44</v>
-      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
@@ -2841,10 +2849,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
@@ -2859,10 +2867,10 @@
         <v>54</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
@@ -2876,8 +2884,12 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="27"/>
+      <c r="B69" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>45</v>
+      </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
@@ -2890,12 +2902,8 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C70" s="27" t="s">
-        <v>50</v>
-      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
@@ -2909,10 +2917,10 @@
         <v>57</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
@@ -2927,10 +2935,10 @@
         <v>58</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C72" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
@@ -2945,10 +2953,10 @@
         <v>59</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="34" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
@@ -2962,8 +2970,12 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="27"/>
+      <c r="B74" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
@@ -2976,12 +2988,8 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B75" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>86</v>
-      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
@@ -2995,10 +3003,10 @@
         <v>62</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C76" s="27" t="s">
-        <v>42</v>
+        <v>82</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25"/>
@@ -3013,10 +3021,10 @@
         <v>63</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
@@ -3031,10 +3039,10 @@
         <v>64</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C78" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="C78" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="D78" s="25"/>
       <c r="E78" s="25"/>
@@ -3048,8 +3056,12 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="27"/>
+      <c r="B79" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>87</v>
+      </c>
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
       <c r="F79" s="25"/>
@@ -3062,12 +3074,8 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B80" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>17</v>
-      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="25"/>
       <c r="E80" s="25"/>
       <c r="F80" s="25"/>
@@ -3077,14 +3085,14 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="22">
-        <f t="shared" ref="A81:A111" si="1">A80+1</f>
+        <f t="shared" ref="A81:A112" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>157</v>
+        <v>21</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
@@ -3098,26 +3106,32 @@
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B82" s="28"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="31"/>
-      <c r="I82" s="32"/>
+      <c r="B82" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="25"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="17"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="22">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B83" s="28"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="30"/>
+      <c r="G83" s="30"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="32"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="22">
@@ -3125,10 +3139,10 @@
         <v>70</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3137,10 +3151,10 @@
         <v>71</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3149,10 +3163,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3161,10 +3175,10 @@
         <v>73</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3173,10 +3187,10 @@
         <v>74</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3185,10 +3199,10 @@
         <v>75</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3197,10 +3211,10 @@
         <v>76</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>162</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3209,10 +3223,10 @@
         <v>77</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3221,10 +3235,10 @@
         <v>78</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3233,10 +3247,10 @@
         <v>79</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3245,7 +3259,7 @@
         <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>78</v>
@@ -3257,10 +3271,10 @@
         <v>81</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3269,7 +3283,7 @@
         <v>82</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>92</v>
@@ -3281,10 +3295,10 @@
         <v>83</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -3293,7 +3307,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>93</v>
@@ -3304,18 +3318,18 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="22">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="22">
@@ -3323,10 +3337,10 @@
         <v>87</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3335,10 +3349,10 @@
         <v>88</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3347,10 +3361,10 @@
         <v>89</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3359,10 +3373,10 @@
         <v>90</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -3371,10 +3385,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -3383,10 +3397,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3394,18 +3408,18 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
+      <c r="B107" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="22">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="22">
@@ -3413,10 +3427,10 @@
         <v>95</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3424,16 +3438,28 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
+      <c r="B110" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="22">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B111" s="1" t="s">
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="22">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3445,7 +3471,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D108:D109 D103:D106" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D109:D110 D104:D107" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
First implementation of Primitive Request body and array request body.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorKtResourceBundle.xlsx
+++ b/meta/program/BlancoRestGeneratorKtResourceBundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8101E907-7563-0C43-8363-193E507FAB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C49FDA-7C3F-A54C-AFCE-AAF60BB68278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="27640" windowHeight="19980" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="187">
   <si>
     <t>リソースバンドル定義書</t>
   </si>
@@ -1061,6 +1061,38 @@
     </rPh>
     <rPh sb="18" eb="20">
       <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BLANCOREST.ERROR.MSG.11</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>電文のペイロードにはプリミティブ型 [{0}] が期待されていますが電文定義・一覧にクエリ文字列以外のプロパティが存在します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニュウリョクデンブｎ </t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t xml:space="preserve">ガタ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">キタイ </t>
+    </rPh>
+    <rPh sb="34" eb="38">
+      <t xml:space="preserve">デンブンテイギ </t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t xml:space="preserve">イチラｎ </t>
+    </rPh>
+    <rPh sb="45" eb="48">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">イガイノ </t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t xml:space="preserve">ソンザイシマス </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1927,10 +1959,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3204,7 +3236,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="21">
-        <f t="shared" ref="A81:A120" si="1">A80+1</f>
+        <f t="shared" ref="A81:A121" si="1">A80+1</f>
         <v>67</v>
       </c>
       <c r="B81" s="22" t="s">
@@ -3574,18 +3606,18 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
+      <c r="B111" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="21">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="21">
@@ -3593,10 +3625,10 @@
         <v>99</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3604,18 +3636,18 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
+      <c r="B114" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="21">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="21">
@@ -3623,10 +3655,10 @@
         <v>102</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3635,10 +3667,10 @@
         <v>103</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3647,10 +3679,10 @@
         <v>104</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3659,10 +3691,10 @@
         <v>105</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3671,9 +3703,21 @@
         <v>106</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="21">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3685,7 +3729,7 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D112:D113 D104:D110" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D113:D114 D104:D111" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>